<commit_message>
add - management command - generate excel dummy transactions
</commit_message>
<xml_diff>
--- a/core/seed_purchases_purchasereceivedetail.xlsx
+++ b/core/seed_purchases_purchasereceivedetail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan.cheng\Documents\Visual Studio Code\Django\p_sys01_repo01\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BFE150-BECC-4C6C-966A-565A6E74129E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADBB175-A66A-42B2-8BEA-EB0586C92B40}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>HEADER CODE</t>
   </si>
@@ -31,19 +31,43 @@
     <t>QUANTITY</t>
   </si>
   <si>
-    <t>PV 003</t>
-  </si>
-  <si>
-    <t>PV 005</t>
-  </si>
-  <si>
-    <t>P REV 01</t>
-  </si>
-  <si>
-    <t>P REV 02</t>
-  </si>
-  <si>
-    <t>PV 001</t>
+    <t>P-REC-1</t>
+  </si>
+  <si>
+    <t>PV-001</t>
+  </si>
+  <si>
+    <t>PV-002</t>
+  </si>
+  <si>
+    <t>PV-003</t>
+  </si>
+  <si>
+    <t>P-REC-2</t>
+  </si>
+  <si>
+    <t>P-REC-3</t>
+  </si>
+  <si>
+    <t>P-REC-4</t>
+  </si>
+  <si>
+    <t>P-REC-5</t>
+  </si>
+  <si>
+    <t>P-REC-6</t>
+  </si>
+  <si>
+    <t>P-REC-7</t>
+  </si>
+  <si>
+    <t>P-REC-8</t>
+  </si>
+  <si>
+    <t>P-REC-9</t>
+  </si>
+  <si>
+    <t>P-REC-10</t>
   </si>
 </sst>
 </file>
@@ -884,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,46 +934,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
       <c r="C4">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>500</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>